<commit_message>
Updates for error handling
</commit_message>
<xml_diff>
--- a/Documents/Test Plan and Results/TestPlan_K9.xlsx
+++ b/Documents/Test Plan and Results/TestPlan_K9.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="96">
   <si>
     <t>Input</t>
   </si>
@@ -269,16 +269,59 @@
     <t>{"callStatus":0}</t>
   </si>
   <si>
-    <t>database down</t>
-  </si>
-  <si>
-    <t>username already exists</t>
-  </si>
-  <si>
-    <t>wrong password</t>
-  </si>
-  <si>
-    <t>wong username (doesn't exist)</t>
+    <t>{"callStatus":2}</t>
+  </si>
+  <si>
+    <t>K9TestResults__16TestOrderProcessService_userNameNotUnique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"callStatus":2}
+</t>
+  </si>
+  <si>
+    <t>{"callStatus":2}
+(The user name is not unique.  Please enter a different user name.)</t>
+  </si>
+  <si>
+    <t>_16TestOrderProcessService _userNameNotUnique</t>
+  </si>
+  <si>
+    <t>{"callStatus":1}</t>
+  </si>
+  <si>
+    <t>_17TestOrderProcessService_wrongPassword</t>
+  </si>
+  <si>
+    <t>accountName="mbp", password="password1"</t>
+  </si>
+  <si>
+    <t>{"callStatus":1}
+(Invalid user name or password.  Try again.)</t>
+  </si>
+  <si>
+    <t>accountName="mbp1", password="password"</t>
+  </si>
+  <si>
+    <t>_18TestOrderProcessService_wrongUserName</t>
+  </si>
+  <si>
+    <t>K9TestResults__17TestOrderProcessService_wrongPassword</t>
+  </si>
+  <si>
+    <t>K9TestResults__18TestOrderProcessService_wrongUserName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TestCDDAO_getCategoryList Test Result: {"callStatus":1000}
+getProductList:{"callStatus":1000}
+getProductInfo:{"callStatus":1000}
+getProductListByCategory:{"callStatus":1000}
+</t>
+  </si>
+  <si>
+    <t>K9TestResults__19TestProductCatalogService_databaseDown</t>
+  </si>
+  <si>
+    <t>_19TestProductCatalogService_databaseDown</t>
   </si>
 </sst>
 </file>
@@ -351,9 +394,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -371,14 +411,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1157,8 +1200,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1167,7 +1210,7 @@
     <col min="2" max="2" width="33.28515625" customWidth="1"/>
     <col min="3" max="3" width="73.85546875" customWidth="1"/>
     <col min="4" max="4" width="95.85546875" customWidth="1"/>
-    <col min="5" max="5" width="43.85546875" customWidth="1"/>
+    <col min="5" max="5" width="61.5703125" customWidth="1"/>
     <col min="6" max="6" width="72.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1184,237 +1227,237 @@
       <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="370.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5" t="s">
+      <c r="B2" s="4"/>
+      <c r="C2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5" t="s">
+      <c r="B3" s="4"/>
+      <c r="C3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="135" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="6"/>
-      <c r="F5" s="5" t="s">
+      <c r="E5" s="5"/>
+      <c r="F5" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="6" t="s">
+      <c r="C6" s="7"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="6" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>60</v>
       </c>
       <c r="D7" s="2"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="7" t="s">
+      <c r="E7" s="5"/>
+      <c r="F7" s="6" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>61</v>
       </c>
       <c r="D8" s="2"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="7" t="s">
+      <c r="E8" s="5"/>
+      <c r="F8" s="6" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>62</v>
       </c>
       <c r="D9" s="2"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="7" t="s">
+      <c r="E9" s="5"/>
+      <c r="F9" s="6" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="315" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="4" t="s">
         <v>65</v>
       </c>
       <c r="D10" s="2"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="5" t="s">
+      <c r="E10" s="5"/>
+      <c r="F10" s="4" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F11" s="4" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="4" t="s">
         <v>63</v>
       </c>
       <c r="D12" s="2"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="7" t="s">
+      <c r="E12" s="5"/>
+      <c r="F12" s="6" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="145.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="4" t="s">
         <v>71</v>
       </c>
       <c r="D13" s="2"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="5" t="s">
+      <c r="E13" s="5"/>
+      <c r="F13" s="4" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="135" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="4" t="s">
         <v>72</v>
       </c>
       <c r="D14" s="2"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="5" t="s">
+      <c r="E14" s="5"/>
+      <c r="F14" s="4" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="4" t="s">
         <v>52</v>
       </c>
       <c r="B15" s="10" t="s">
@@ -1422,53 +1465,102 @@
       </c>
       <c r="C15" s="11"/>
       <c r="D15" s="11"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="7" t="s">
+      <c r="E15" s="5"/>
+      <c r="F15" s="6" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="228.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="4" t="s">
         <v>74</v>
       </c>
       <c r="D16" s="2"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="7" t="s">
+      <c r="E16" s="5"/>
+      <c r="F16" s="6" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="315" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D17" t="s">
         <v>80</v>
       </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+      <c r="E17" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="12" t="s">
+      <c r="F17" s="3" t="s">
         <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D18" t="s">
+        <v>85</v>
+      </c>
+      <c r="E18" t="s">
+        <v>91</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D19" t="s">
+        <v>85</v>
+      </c>
+      <c r="E19" t="s">
+        <v>92</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E20" t="s">
+        <v>94</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1508,10 +1600,10 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="3"/>
+      <c r="C2" s="12"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">

</xml_diff>

<commit_message>
Fixed some interface issues after testing with SoapUI
</commit_message>
<xml_diff>
--- a/Documents/Test Plan and Results/TestPlan_K9.xlsx
+++ b/Documents/Test Plan and Results/TestPlan_K9.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="JUnit tests" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="128">
   <si>
     <t>Input</t>
   </si>
@@ -322,6 +322,102 @@
   </si>
   <si>
     <t>_19TestProductCatalogService_databaseDown</t>
+  </si>
+  <si>
+    <t>getAccount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   &lt;soapenv:Header/&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      &lt;ord:getAccount&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         &lt;ord:accountName&gt;{"accountName":"mbp"}&lt;/ord:accountName&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         &lt;ord:password&gt;{"password":"password"}&lt;/ord:password&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      &lt;/ord:getAccount&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      &lt;getAccountResponse xmlns="http://OrderProcessService.WebServices.K9.com"&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         &lt;getAccountReturn&gt;{"accountId":1,"accountName":"mbp","password1":"1000:b3e45d005222ba534b12e4dfa9230e0d378a62d04529c76d:d536bb2e96025614dfe826c19325fbeda7d1ff0df517ecc0","fName":"Michele","lName":"Belanger","billingAddressId":1,"shippingAddressId":2,"email":"mbp@gmail.com"}&lt;/getAccountReturn&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      &lt;/getAccountResponse&gt;</t>
+  </si>
+  <si>
+    <t>createAccount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      &lt;ord:creatAccount&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      &lt;/ord:creatAccount&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      &lt;creatAccountResponse xmlns="http://OrderProcessService.WebServices.K9.com"&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      &lt;/creatAccountResponse&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         &lt;creatAccountReturn&gt;{"callStatus":0}&lt;/creatAccountReturn&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ord:accountInfo&gt;{"accountName":"mbp","password1":"password","fName":"michele","lName":"belanger","billingAddressId":0,"shippingAddressId":0,"email":"mbp@gmail.com","billingAddressStreet":"235 Oak av","billingAddressCity":"Perth","billingAddressProvince":"ON","billingAddressCountry":"Canada","billingAddressPostalCode":"K0A 8F9","billingAddressPhone":"613 235-4875","shippingAddressStreet":"2564 Maple drive","shippingAddressCity":"Ottawa","shippingAddressProvince":"ON","shippingAddressCountry":"Canada","shippingAddressPostalCode":"K4R6T5","shippingAddressPhone":"613 856-7458"}&lt;/ord:accountInfo&gt;</t>
+  </si>
+  <si>
+    <t>createOrder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      &lt;ord:createOrder&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         &lt;ord:shoppingCartInfo&gt;[{"orderId":1,"cdid":1,"quantity":3},{"orderId":1,"cdid":2,"quantity":2}]&lt;/ord:shoppingCartInfo&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         &lt;ord:shippingInfo&gt;{"accountId":1,"shippingCharge":5.25,"taxes":4.25,"totalCost":50.32}&lt;/ord:shippingInfo&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      &lt;/ord:createOrder&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      &lt;createOrderResponse xmlns="http://OrderProcessService.WebServices.K9.com"&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         &lt;createOrderReturn&gt;{"callStatus":0}&lt;/createOrderReturn&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      &lt;/createOrderResponse&gt;</t>
+  </si>
+  <si>
+    <t>confirmOrder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      &lt;ord:confirmOrder&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         &lt;ord:purchaseOrder&gt;{"orderId":1,"accountId":1,"status":"ORDERED","shippingCharge":5.2,"taxes":6.2,"totalCost":20.36}&lt;/ord:purchaseOrder&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         &lt;ord:paymentInfo&gt;{"creditCardHolderName":"MBP","creditCardNumber":"4538452625981254","expiryDate":"12/2018","ccv":235&lt;/ord:paymentInfo&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      &lt;/ord:confirmOrder&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      &lt;confirmOrderResponse xmlns="http://OrderProcessService.WebServices.K9.com"&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         &lt;confirmOrderReturn&gt;{"callStatus":0}&lt;/confirmOrderReturn&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      &lt;/confirmOrderResponse&gt;</t>
   </si>
 </sst>
 </file>
@@ -1200,7 +1296,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+    <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
@@ -1575,10 +1671,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1769,11 +1865,222 @@
         <v>11</v>
       </c>
     </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>96</v>
+      </c>
+      <c r="C34" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>97</v>
+      </c>
+      <c r="C35" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>9</v>
+      </c>
+      <c r="C36" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>98</v>
+      </c>
+      <c r="C37" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>99</v>
+      </c>
+      <c r="C38" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B44" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C44" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B45" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C45" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B46" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C46" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C47" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B48" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C48" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B49" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B53" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C53" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B54" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C54" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="B55" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C55" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="B56" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C56" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B57" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C57" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B58" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B62" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C62" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B63" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C63" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="B64" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C64" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="B65" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C65" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="B66" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C66" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B67" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B68" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:C2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
update with changes made during meeting
</commit_message>
<xml_diff>
--- a/Documents/Test Plan and Results/TestPlan_K9.xlsx
+++ b/Documents/Test Plan and Results/TestPlan_K9.xlsx
@@ -1673,8 +1673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="C56" sqref="C56"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1758,11 +1758,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="255" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>16</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="1" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1798,11 +1798,11 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>30</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="1" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update interface definition calls in excel spreadsheet - SOAPUI tab
</commit_message>
<xml_diff>
--- a/Documents/Test Plan and Results/TestPlan_K9.xlsx
+++ b/Documents/Test Plan and Results/TestPlan_K9.xlsx
@@ -378,21 +378,12 @@
     <t xml:space="preserve">      &lt;ord:createOrder&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">         &lt;ord:shoppingCartInfo&gt;[{"orderId":1,"cdid":1,"quantity":3},{"orderId":1,"cdid":2,"quantity":2}]&lt;/ord:shoppingCartInfo&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">         &lt;ord:shippingInfo&gt;{"accountId":1,"shippingCharge":5.25,"taxes":4.25,"totalCost":50.32}&lt;/ord:shippingInfo&gt;</t>
-  </si>
-  <si>
     <t xml:space="preserve">      &lt;/ord:createOrder&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">      &lt;createOrderResponse xmlns="http://OrderProcessService.WebServices.K9.com"&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">         &lt;createOrderReturn&gt;{"callStatus":0}&lt;/createOrderReturn&gt;</t>
-  </si>
-  <si>
     <t xml:space="preserve">      &lt;/createOrderResponse&gt;</t>
   </si>
   <si>
@@ -402,9 +393,6 @@
     <t xml:space="preserve">      &lt;ord:confirmOrder&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">         &lt;ord:purchaseOrder&gt;{"orderId":1,"accountId":1,"status":"ORDERED","shippingCharge":5.2,"taxes":6.2,"totalCost":20.36}&lt;/ord:purchaseOrder&gt;</t>
-  </si>
-  <si>
     <t xml:space="preserve">         &lt;ord:paymentInfo&gt;{"creditCardHolderName":"MBP","creditCardNumber":"4538452625981254","expiryDate":"12/2018","ccv":235&lt;/ord:paymentInfo&gt;</t>
   </si>
   <si>
@@ -418,6 +406,18 @@
   </si>
   <si>
     <t xml:space="preserve">      &lt;/confirmOrderResponse&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         &lt;ord:shoppingCartInfo&gt;[{"accountName":"mbp","cdid":1,"quantity":3},{"accountName":"mbp","cdid":2,"quantity":2}]&lt;/ord:shoppingCartInfo&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         &lt;ord:shippingInfo&gt;{"accountName":"mbp","shippingCharge":5.25,"taxes":4.25,"totalCost":50.32}&lt;/ord:shippingInfo&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         &lt;createOrderReturn&gt;{"orderId":1}&lt;/createOrderReturn&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         &lt;ord:purchaseOrder&gt;{"orderId":1,"accountId":0,"status":"","shippingCharge":5.2,"taxes":6.2,"totalCost":20.36}&lt;/ord:purchaseOrder&gt;</t>
   </si>
 </sst>
 </file>
@@ -1673,8 +1673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="C70" sqref="C70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1718,11 +1718,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1841,11 +1841,11 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>35</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="1" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1988,28 +1988,28 @@
         <v>113</v>
       </c>
       <c r="C54" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B55" s="1" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
       <c r="C55" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B56" s="1" t="s">
-        <v>115</v>
+        <v>125</v>
       </c>
       <c r="C56" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B57" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C57" t="s">
         <v>11</v>
@@ -2022,12 +2022,12 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B62" s="1" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="C62" t="s">
         <v>17</v>
@@ -2035,31 +2035,31 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B63" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C63" t="s">
         <v>121</v>
-      </c>
-      <c r="C63" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B64" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C64" t="s">
         <v>122</v>
-      </c>
-      <c r="C64" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="65" spans="2:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B65" s="1" t="s">
-        <v>115</v>
+        <v>125</v>
       </c>
       <c r="C65" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="66" spans="2:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B66" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C66" t="s">
         <v>11</v>
@@ -2067,7 +2067,7 @@
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B67" s="1" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated sequence and package diagrams
</commit_message>
<xml_diff>
--- a/Documents/Test Plan and Results/TestPlan_K9.xlsx
+++ b/Documents/Test Plan and Results/TestPlan_K9.xlsx
@@ -1673,8 +1673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="B61" sqref="B61"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
updated test results in excel spreadsheet
</commit_message>
<xml_diff>
--- a/Documents/Test Plan and Results/TestPlan_K9.xlsx
+++ b/Documents/Test Plan and Results/TestPlan_K9.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600"/>
   </bookViews>
   <sheets>
     <sheet name="JUnit tests" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="136">
   <si>
     <t>Input</t>
   </si>
@@ -61,9 +61,6 @@
   </si>
   <si>
     <t xml:space="preserve">      &lt;/getCategoryListResponse&gt;</t>
-  </si>
-  <si>
-    <t>http://localhost:8080/CDStore/services/ProductCatalogService?wsdl</t>
   </si>
   <si>
     <t>getCategoryList</t>
@@ -235,9 +232,6 @@
     <t>_12TestOrderProcessService_createOrder</t>
   </si>
   <si>
-    <t>[{"accountName":"mbp","cdid":"1","quantity":"3"},{"accountName":"mbp","cdid":"2","quantity":"2"}], {"accountId":1,"shippingCharge":7.25,"taxes":5.25,"totalCost":60.32}</t>
-  </si>
-  <si>
     <t>orders table:
 accountId=1, status="ordered", shippingCharge=7.25, taxes=5.25, totalCost=60.32
 orderItem table:
@@ -419,12 +413,43 @@
   <si>
     <t xml:space="preserve">         &lt;getAccountReturn&gt;{"accountName":"mbp","password1":"","fName":"michele","lName":"belanger","billingAddressId":1,"shippingAddressId":2,"email":"mbp@gmail.com"}&lt;/getAccountReturn&gt;</t>
   </si>
+  <si>
+    <t>K9TestResults__9TestOrderProcessService_createAccount</t>
+  </si>
+  <si>
+    <t>{"accountName":"mbp","password1":"","fName":"Michele","lName":"Belanger","billingAddressId":1,"shippingAddressId":2,"email":"mbp@gmail.com"}</t>
+  </si>
+  <si>
+    <t>K9TestResults__10TestOrderProcessService_getAccount</t>
+  </si>
+  <si>
+    <t>[{"accountName":"mbp","cdid":"1","quantity":"3"},{"accountName":"mbp","cdid":"2","quantity":"2"}],
+{"accountName":"mbp","shippingCharge":7.25,"taxes":5.25,"totalCost":60.32}</t>
+  </si>
+  <si>
+    <t>K9TestResults__12TestOrderProcessService_createOrder</t>
+  </si>
+  <si>
+    <t>{"orderId":1}</t>
+  </si>
+  <si>
+    <t>{"orderId":1,"accountId":1,"status":"ORDERED","shippingCharge":7.25,"taxes":5.25,"totalCost":60.32},{"accountName":"mbp","shippingCharge":7.25,"taxes":5.25,"totalCost":60.32}, {"creditCardHolderName":"MBP","creditCardNumber":"4538452625981254","expiryDate":"12/2018","ccv":235}</t>
+  </si>
+  <si>
+    <t>K9TestResults__13TestOrderProcessService_confirmOrder</t>
+  </si>
+  <si>
+    <t>K9TestResults__14TestOrderProcessService_orderProcessTest</t>
+  </si>
+  <si>
+    <t>K9TestResults__15TestOrderProcessService_DenyEveryFifthConfirmRequest</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -439,8 +464,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -452,8 +484,13 @@
         <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -476,21 +513,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -507,9 +557,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -519,10 +566,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="2" builtinId="10"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -1296,8 +1354,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1312,7 +1370,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -1323,340 +1381,351 @@
       <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="F1" s="6" t="s">
+      <c r="E1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="370.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="F5" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="5" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="370.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="135" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+    <row r="8" spans="1:6" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="F6" s="6" t="s">
+      <c r="B8" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="315" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="6" t="s">
+    <row r="11" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="145.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="228.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="315" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="315" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="4" t="s">
+      <c r="E17" s="4" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="145.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="D13" s="2"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="135" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="6" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="228.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="D16" s="2"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="6" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="315" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="D17" t="s">
-        <v>80</v>
-      </c>
-      <c r="E17" s="3" t="s">
+      <c r="F17" s="3" t="s">
         <v>81</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="F18" s="3" t="s">
         <v>86</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="D18" t="s">
-        <v>85</v>
-      </c>
-      <c r="E18" t="s">
-        <v>91</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E19" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="D19" t="s">
-        <v>85</v>
-      </c>
-      <c r="E19" t="s">
+      <c r="F19" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E20" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="F19" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="E20" t="s">
-        <v>94</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>77</v>
+      <c r="F20" s="5" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1673,8 +1742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1686,28 +1755,26 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
         <v>22</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>23</v>
       </c>
-      <c r="C1" t="s">
-        <v>24</v>
-      </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B2" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="12"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1723,7 +1790,7 @@
         <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1739,15 +1806,17 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B8" s="1"/>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="11"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="11"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1755,15 +1824,15 @@
         <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="255" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -1771,7 +1840,7 @@
         <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -1779,39 +1848,44 @@
         <v>11</v>
       </c>
     </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="11"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+    </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1822,39 +1896,44 @@
         <v>11</v>
       </c>
     </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="11"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+    </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C26" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C29" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -1865,20 +1944,25 @@
         <v>11</v>
       </c>
     </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="11"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="11"/>
+    </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C34" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C35" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -1886,20 +1970,20 @@
         <v>9</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C37" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C38" t="s">
         <v>11</v>
@@ -1907,12 +1991,12 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -1920,46 +2004,51 @@
         <v>11</v>
       </c>
     </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="11"/>
+      <c r="B42" s="11"/>
+      <c r="C42" s="11"/>
+    </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B44" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C44" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B45" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C45" t="s">
         <v>105</v>
-      </c>
-      <c r="C45" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B46" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C46" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C47" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B48" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C48" t="s">
         <v>11</v>
@@ -1970,46 +2059,51 @@
         <v>11</v>
       </c>
     </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="11"/>
+      <c r="B51" s="11"/>
+      <c r="C51" s="11"/>
+    </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B53" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C53" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B54" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C54" t="s">
         <v>112</v>
-      </c>
-      <c r="C54" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B55" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C55" t="s">
         <v>123</v>
-      </c>
-      <c r="C55" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B56" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C56" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B57" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C57" t="s">
         <v>11</v>
@@ -2020,46 +2114,51 @@
         <v>11</v>
       </c>
     </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="11"/>
+      <c r="B60" s="11"/>
+      <c r="C60" s="11"/>
+    </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B62" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C62" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B63" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C63" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B64" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C64" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="65" spans="2:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B65" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C65" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="66" spans="2:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B66" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C66" t="s">
         <v>11</v>
@@ -2067,7 +2166,7 @@
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B67" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.25">

</xml_diff>